<commit_message>
User can now specify which channels to use for clustering beads data.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="beads" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>File Path</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>None, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
+  </si>
+  <si>
+    <t>Clustering Channels</t>
+  </si>
+  <si>
+    <t>FL1-H, FL2-H, FL3-H</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +447,10 @@
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -456,8 +463,11 @@
       <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -469,6 +479,9 @@
       </c>
       <c r="D2" t="s">
         <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added support for multiple channels and transformations, Fixed #25, Fixed #8, Fixed #30
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\OneDrive\Work\TaborLab\Code\fc\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="beads" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>File Path</t>
   </si>
@@ -49,9 +49,6 @@
     <t>FCFiles/data.005</t>
   </si>
   <si>
-    <t>MEFL</t>
-  </si>
-  <si>
     <t>FCFiles/data.006</t>
   </si>
   <si>
@@ -71,6 +68,21 @@
   </si>
   <si>
     <t>FL1-H, FL2-H, FL3-H</t>
+  </si>
+  <si>
+    <t>FL1-H Peaks</t>
+  </si>
+  <si>
+    <t>FL1-H Transform</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Exponential</t>
+  </si>
+  <si>
+    <t>Mef</t>
   </si>
 </sst>
 </file>
@@ -437,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,33 +467,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0.3</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -492,21 +504,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -514,94 +527,109 @@
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2">
         <v>0.3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="b">
+      <c r="F2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.1</v>
       </c>
-      <c r="E3" s="2" t="b">
+      <c r="F3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2" t="b">
+      <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.25</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="b">
+      <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trimming now operates on non-transformed data
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>File Path</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Mef</t>
+  </si>
+  <si>
+    <t>FL2-H Transform</t>
   </si>
 </sst>
 </file>
@@ -504,22 +507,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="4" width="15.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -530,33 +533,36 @@
         <v>17</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0.3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="b">
+      <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -566,17 +572,17 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.1</v>
       </c>
-      <c r="F3" s="2" t="b">
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -586,17 +592,17 @@
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.5</v>
       </c>
-      <c r="F4" s="2" t="b">
+      <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -606,17 +612,20 @@
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="b">
+      <c r="G5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -626,10 +635,10 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Supports Mef calculations for all bead channels
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -15,12 +15,12 @@
     <sheet name="beads" sheetId="2" r:id="rId1"/>
     <sheet name="cells" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" calcOnSave="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>File Path</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>FL2-H Transform</t>
+  </si>
+  <si>
+    <t>FL3-H Peaks</t>
+  </si>
+  <si>
+    <t>FL3-H Transform</t>
   </si>
 </sst>
 </file>
@@ -450,22 +456,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -473,29 +480,35 @@
         <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
         <v>0.3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -507,22 +520,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="5" width="15.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -536,33 +549,36 @@
         <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="b">
+      <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -572,17 +588,17 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.1</v>
       </c>
-      <c r="G3" s="2" t="b">
+      <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -592,17 +608,17 @@
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.5</v>
       </c>
-      <c r="G4" s="2" t="b">
+      <c r="H4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -615,17 +631,17 @@
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.25</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="b">
+      <c r="H5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -635,10 +651,13 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Supports fcs3 in run_excel, removes support for fcs2
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -15,12 +15,12 @@
     <sheet name="beads" sheetId="2" r:id="rId1"/>
     <sheet name="cells" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>File Path</t>
   </si>
@@ -28,54 +28,21 @@
     <t>Gate Fraction</t>
   </si>
   <si>
-    <t>Kinase</t>
-  </si>
-  <si>
     <t>Beads File Path</t>
   </si>
   <si>
-    <t>FCFiles/data.001</t>
-  </si>
-  <si>
-    <t>FCFiles/data.002</t>
-  </si>
-  <si>
-    <t>FCFiles/data.003</t>
-  </si>
-  <si>
-    <t>FCFiles/data.004</t>
-  </si>
-  <si>
-    <t>FCFiles/data.005</t>
-  </si>
-  <si>
-    <t>FCFiles/data.006</t>
-  </si>
-  <si>
     <t>Clustering Method</t>
   </si>
   <si>
     <t>gmm</t>
   </si>
   <si>
-    <t>aTc</t>
-  </si>
-  <si>
     <t>None, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
   </si>
   <si>
     <t>Clustering Channels</t>
   </si>
   <si>
-    <t>FL1-H, FL2-H, FL3-H</t>
-  </si>
-  <si>
-    <t>FL1-H Peaks</t>
-  </si>
-  <si>
-    <t>FL1-H Transform</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -85,13 +52,40 @@
     <t>Mef</t>
   </si>
   <si>
-    <t>FL2-H Transform</t>
-  </si>
-  <si>
-    <t>FL3-H Peaks</t>
-  </si>
-  <si>
-    <t>FL3-H Transform</t>
+    <t>FCFiles/data_001.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data_002.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data_003.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data_004.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data_005.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data_006.fcs</t>
+  </si>
+  <si>
+    <t>FL1 Transform</t>
+  </si>
+  <si>
+    <t>FL2 Transform</t>
+  </si>
+  <si>
+    <t>FL3 Transform</t>
+  </si>
+  <si>
+    <t>FL1 Peaks</t>
+  </si>
+  <si>
+    <t>FL3 Peaks</t>
+  </si>
+  <si>
+    <t>FL1, FL2, FL3</t>
   </si>
 </sst>
 </file>
@@ -135,11 +129,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -147,10 +138,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +446,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,43 +460,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.3</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -520,145 +507,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.3</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split excel file into a test and template file, fixes #45
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="beads" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>File Path</t>
   </si>
@@ -449,17 +449,17 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -510,18 +510,18 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -541,24 +541,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -566,7 +560,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -580,7 +574,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -597,7 +591,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Corrected mistake in experiment.xlsx.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\OneDrive\Work\TaborLab\Code\fc\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\castillohair\Documents\Rice\Lab\Programs\fc\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="beads" sheetId="2" r:id="rId1"/>
@@ -449,17 +449,17 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -510,18 +510,18 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -541,15 +541,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -560,7 +563,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -574,7 +577,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -591,7 +594,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Eliminated excel_io, updated examples/experiment.xlsx, and redirected test_excel_ui to it.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -2,54 +2,173 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\castillohair\Documents\Rice\Lab\Programs\fc\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="beads" sheetId="2" r:id="rId1"/>
-    <sheet name="cells" sheetId="1" r:id="rId2"/>
+    <sheet name="Instruments" sheetId="1" r:id="rId1"/>
+    <sheet name="Beads" sheetId="2" r:id="rId2"/>
+    <sheet name="Samples" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Forward Scatter Channel</t>
+  </si>
+  <si>
+    <t>Side Scatter Channel</t>
+  </si>
+  <si>
+    <t>Time Channel</t>
+  </si>
+  <si>
+    <t>Fluorescence Channels</t>
+  </si>
+  <si>
+    <t>Moake's Flow Cytometer</t>
+  </si>
+  <si>
+    <t>Moake's Flow Cytometer (new acquisition card)</t>
+  </si>
+  <si>
+    <t>FSC-H</t>
+  </si>
+  <si>
+    <t>SSC-H</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>FL1-H, FL2-H, FL3-H</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>FSC</t>
+  </si>
+  <si>
+    <t>SSC</t>
+  </si>
+  <si>
+    <t>FL1, FL2, FL3</t>
+  </si>
+  <si>
+    <t>Instrument ID</t>
+  </si>
   <si>
     <t>File Path</t>
   </si>
   <si>
+    <t>FL1 MEF Values</t>
+  </si>
+  <si>
     <t>Gate Fraction</t>
   </si>
   <si>
-    <t>Beads File Path</t>
-  </si>
-  <si>
-    <t>Clustering Method</t>
-  </si>
-  <si>
-    <t>gmm</t>
-  </si>
-  <si>
-    <t>None, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
+    <t>Lot</t>
   </si>
   <si>
     <t>Clustering Channels</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Exponential</t>
-  </si>
-  <si>
-    <t>Mef</t>
+    <t>AF02</t>
+  </si>
+  <si>
+    <t>0, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
+  </si>
+  <si>
+    <t>FL1-H</t>
+  </si>
+  <si>
+    <t>FL1, FL3</t>
+  </si>
+  <si>
+    <t>Beads ID</t>
+  </si>
+  <si>
+    <t>Strain name</t>
+  </si>
+  <si>
+    <t>IPTG (µM)</t>
+  </si>
+  <si>
+    <t>S0001</t>
+  </si>
+  <si>
+    <t>B0001</t>
+  </si>
+  <si>
+    <t>B0002</t>
+  </si>
+  <si>
+    <t>FC001</t>
+  </si>
+  <si>
+    <t>FC002</t>
+  </si>
+  <si>
+    <t>S0002</t>
+  </si>
+  <si>
+    <t>S0003</t>
+  </si>
+  <si>
+    <t>S0004</t>
+  </si>
+  <si>
+    <t>S0005</t>
+  </si>
+  <si>
+    <t>S0006</t>
+  </si>
+  <si>
+    <t>sSC0001</t>
+  </si>
+  <si>
+    <t>FL1 Units</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>MEF</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>FCFiles/data_006.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/data.006</t>
+  </si>
+  <si>
+    <t>FCFiles/data.001</t>
+  </si>
+  <si>
+    <t>FCFiles/data.002</t>
+  </si>
+  <si>
+    <t>FCFiles/data.003</t>
+  </si>
+  <si>
+    <t>FCFiles/data.004</t>
+  </si>
+  <si>
+    <t>FCFiles/data.005</t>
   </si>
   <si>
     <t>FCFiles/data_001.fcs</t>
@@ -67,25 +186,25 @@
     <t>FCFiles/data_005.fcs</t>
   </si>
   <si>
-    <t>FCFiles/data_006.fcs</t>
-  </si>
-  <si>
-    <t>FL1 Transform</t>
-  </si>
-  <si>
-    <t>FL2 Transform</t>
-  </si>
-  <si>
-    <t>FL3 Transform</t>
-  </si>
-  <si>
-    <t>FL1 Peaks</t>
-  </si>
-  <si>
-    <t>FL3 Peaks</t>
-  </si>
-  <si>
-    <t>FL1, FL2, FL3</t>
+    <t>S0007</t>
+  </si>
+  <si>
+    <t>S0008</t>
+  </si>
+  <si>
+    <t>S0009</t>
+  </si>
+  <si>
+    <t>S0010</t>
+  </si>
+  <si>
+    <t>S0011</t>
+  </si>
+  <si>
+    <t>FL1-H Units</t>
+  </si>
+  <si>
+    <t>FL1-H MEF Values</t>
   </si>
 </sst>
 </file>
@@ -103,7 +222,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,25 +245,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -443,176 +557,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.3</v>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>0.3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11">
+        <v>0.3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added stats reporting to excel_ui.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +934,7 @@
         <v>41</v>
       </c>
       <c r="G8">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H8" t="s">
         <v>39</v>
@@ -957,7 +957,7 @@
         <v>43</v>
       </c>
       <c r="G9">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
@@ -983,7 +983,7 @@
         <v>42</v>
       </c>
       <c r="G10">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="H10" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Added more channels to experiment.xlsx.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>FL1-H MEF Values</t>
+  </si>
+  <si>
+    <t>FL2 Units</t>
+  </si>
+  <si>
+    <t>FL3 Units</t>
+  </si>
+  <si>
+    <t>FL3 MEF Values</t>
+  </si>
+  <si>
+    <t>0, 1614, 4035, 12025, 31896, 95682, 353225, 1077421</t>
   </si>
 </sst>
 </file>
@@ -640,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,11 +665,12 @@
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,13 +690,16 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -699,14 +715,14 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -722,10 +738,13 @@
       <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3">
         <v>0.3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -736,9 +755,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -748,12 +767,13 @@
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,16 +793,22 @@
         <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -792,17 +818,17 @@
       <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -815,17 +841,17 @@
       <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -838,17 +864,17 @@
       <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -864,17 +890,17 @@
       <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -890,17 +916,17 @@
       <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0.3</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>39</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -910,17 +936,17 @@
       <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>0.3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>39</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -933,17 +959,17 @@
       <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0.2</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>39</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -956,17 +982,17 @@
       <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>0.2</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>39</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -982,17 +1008,20 @@
       <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10">
         <v>0.25</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>39</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1008,17 +1037,20 @@
       <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="G11">
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
         <v>0.3</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>39</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1034,13 +1066,13 @@
       <c r="F12" t="s">
         <v>42</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>0.1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>39</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for a.u. in the Excel UI.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
     <sheet name="Beads" sheetId="2" r:id="rId2"/>
     <sheet name="Samples" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" calcOnSave="0"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -147,9 +147,6 @@
     <t>MEF</t>
   </si>
   <si>
-    <t>RFI</t>
-  </si>
-  <si>
     <t>FCFiles/data_006.fcs</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>0, 1614, 4035, 12025, 31896, 95682, 353225, 1077421</t>
+  </si>
+  <si>
+    <t>a.u.</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -684,13 +684,13 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>19</v>
@@ -707,7 +707,7 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -730,7 +730,7 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -739,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <v>0.3</v>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,16 +787,16 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>19</v>
@@ -816,7 +816,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2">
         <v>0.3</v>
@@ -836,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
@@ -859,10 +859,10 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="I4">
         <v>0.3</v>
@@ -885,7 +885,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>42</v>
@@ -911,7 +911,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
@@ -934,7 +934,7 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7">
         <v>0.3</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
@@ -971,16 +971,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="I9">
         <v>0.2</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1003,13 +1003,13 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>0.25</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -1032,7 +1032,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
         <v>42</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -1061,7 +1061,7 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Changed example dataset and scripts.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE69A4E-716F-4542-8EE0-97EE2E6F1BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="6285" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -102,50 +103,122 @@
     <t>Beads Lot</t>
   </si>
   <si>
-    <t>AG01</t>
-  </si>
-  <si>
-    <t>0, 646, 1704, 4827, 15991, 47609, 135896, 273006</t>
-  </si>
-  <si>
-    <t>FCFiles/Beads006.fcs</t>
-  </si>
-  <si>
-    <t>IPTG (mM)</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
-    <t>Plasmid</t>
-  </si>
-  <si>
-    <t>BW29655</t>
-  </si>
-  <si>
-    <t>pSC0012</t>
-  </si>
-  <si>
-    <t>FCFiles/Data001.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/Data002.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/Data003.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/Data004.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/Data005.fcs</t>
+    <t>sJS1123</t>
+  </si>
+  <si>
+    <t>sJS1012</t>
+  </si>
+  <si>
+    <t>sJS1007</t>
+  </si>
+  <si>
+    <t>Plasmids</t>
+  </si>
+  <si>
+    <t>pJS0355, pJS0304, pSC31_3</t>
+  </si>
+  <si>
+    <t>DAPG (uM)</t>
+  </si>
+  <si>
+    <t>pJS0143, pJS0130, pSC31_3</t>
+  </si>
+  <si>
+    <t>pJS0143, pJS0304, pSC31_3</t>
+  </si>
+  <si>
+    <t>S0006</t>
+  </si>
+  <si>
+    <t>S0007</t>
+  </si>
+  <si>
+    <t>S0008</t>
+  </si>
+  <si>
+    <t>S0009</t>
+  </si>
+  <si>
+    <t>S0010</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>AJ01</t>
+  </si>
+  <si>
+    <t>AK02</t>
+  </si>
+  <si>
+    <t>0, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
+  </si>
+  <si>
+    <t>0, 771, 2106, 6262, 15183, 45292, 136258, 291042</t>
+  </si>
+  <si>
+    <t>BMIN</t>
+  </si>
+  <si>
+    <t>BMAX</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample001.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/min/sample001.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/max/sample002.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/min/sample004.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/max/sample008.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample006.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample007.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample008.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample009.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample010.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample011.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample012.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample013.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample014.fcs</t>
+  </si>
+  <si>
+    <t>./FCFiles/sample015.fcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +230,12 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -524,24 +603,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -587,25 +664,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -636,18 +711,64 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F2">
-        <v>0.3</v>
+        <v>0.85</v>
       </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3">
+        <v>0.85</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4">
+        <v>0.85</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -657,29 +778,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,16 +818,16 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -719,25 +838,25 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -748,25 +867,25 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3">
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2.3323619999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -777,25 +896,25 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4">
-        <v>0.161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.3634490000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -806,25 +925,25 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I5">
-        <v>0.318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8.1632650000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -835,25 +954,229 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6">
+        <v>15.272069999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>0.85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7">
+        <v>28.571429999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>0.85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8">
+        <v>53.452249999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>0.85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>0.85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10">
+        <v>187.0829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>0.85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12">
+        <v>0.85</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
         <v>35</v>
       </c>
-      <c r="I6">
-        <v>1</v>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>0.85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated example scripts with new controls.
</commit_message>
<xml_diff>
--- a/examples/experiment.xlsx
+++ b/examples/experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/castillohair/Documents/Programs/FlowCal-recent/FlowCal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC391968-646F-1747-9DEA-7D012B071C0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731AA2EB-F088-C546-92CF-27F59A2882D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="23500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -130,12 +130,6 @@
     <t>pSC31_3, pJS0130, pJS0143</t>
   </si>
   <si>
-    <t>sJS1014</t>
-  </si>
-  <si>
-    <t>pSC31_3, pJS0306, pJS0143</t>
-  </si>
-  <si>
     <t>Autofluorescence control.</t>
   </si>
   <si>
@@ -235,31 +229,37 @@
     <t>FCFiles/sample037.fcs</t>
   </si>
   <si>
-    <t>FCFiles/controls/sample019.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/controls/sample010.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/controls/sample004.fcs</t>
-  </si>
-  <si>
     <t>B004</t>
   </si>
   <si>
     <t>FCFiles/sample001.fcs</t>
   </si>
   <si>
-    <t>FCFiles/controls/sample001.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/controls/sample002.fcs</t>
-  </si>
-  <si>
-    <t>FCFiles/controls/sample003.fcs</t>
-  </si>
-  <si>
     <t>FL1, FL2</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/nfc/sample004.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/nfc/sample003.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/sfc2/sample019.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/sfc2/sample001.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/sfc1/sample003.fcs</t>
+  </si>
+  <si>
+    <t>FCFiles/controls/sfc1/sample007.fcs</t>
+  </si>
+  <si>
+    <t>sJS1061</t>
+  </si>
+  <si>
+    <t>pSC31_3, pJS0306</t>
   </si>
 </sst>
 </file>
@@ -692,7 +692,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -704,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -720,7 +720,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -746,13 +746,13 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -763,13 +763,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -778,24 +778,24 @@
         <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2">
         <v>0.85</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -804,50 +804,50 @@
         <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2">
         <v>0.85</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2">
         <v>0.85</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -856,13 +856,13 @@
         <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5">
         <v>0.85</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +876,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -912,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -932,16 +932,16 @@
     </row>
     <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>17</v>
@@ -956,7 +956,7 @@
         <v>30</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>31</v>
@@ -967,16 +967,16 @@
     </row>
     <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>17</v>
@@ -988,13 +988,13 @@
         <v>0.85</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
@@ -1002,16 +1002,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -1037,16 +1037,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -1072,16 +1072,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
@@ -1107,16 +1107,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
@@ -1142,16 +1142,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
@@ -1177,16 +1177,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>17</v>
@@ -1212,16 +1212,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>17</v>
@@ -1247,16 +1247,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>17</v>
@@ -1282,16 +1282,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>17</v>
@@ -1317,16 +1317,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>17</v>

</xml_diff>